<commit_message>
Updated display with uptime. Needs cleaning up.
</commit_message>
<xml_diff>
--- a/Design/Screen-Layout.xlsx
+++ b/Design/Screen-Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsasala/Development/Aquarius/Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6ECC68-3C50-F64E-A5B0-FE24A843C48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974F8919-9350-654F-9906-069363C30378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23160" yWindow="1980" windowWidth="22960" windowHeight="17440" activeTab="1" xr2:uid="{0158349C-1CEF-DB49-8367-4BA8D3BA6996}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="39">
   <si>
     <t>W</t>
   </si>
@@ -138,6 +138,24 @@
   <si>
     <t>PE</t>
   </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
 </sst>
 </file>
 
@@ -185,7 +203,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -404,24 +422,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -473,15 +478,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1839,8 +1835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE90A50E-CDCD-574E-8857-69572E52BB25}">
   <dimension ref="A1:EA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6038,7 +6034,7 @@
       <c r="V30" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W30" s="23" t="s">
+      <c r="W30" s="10" t="s">
         <v>24</v>
       </c>
       <c r="X30" s="11" t="s">
@@ -6289,59 +6285,59 @@
       <c r="C32" s="4">
         <v>2</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="E32" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F32" s="16" t="s">
+      <c r="F32" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G32" s="16" t="s">
+      <c r="G32" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H32" s="16" t="s">
+      <c r="H32" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16" t="s">
+      <c r="I32" s="13"/>
+      <c r="J32" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K32" s="16">
+      <c r="K32" s="13">
         <v>5</v>
       </c>
-      <c r="L32" s="16">
+      <c r="L32" s="13">
         <v>5</v>
       </c>
-      <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
-      <c r="O32" s="16" t="s">
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="P32" s="16" t="s">
+      <c r="P32" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="Q32" s="16" t="s">
+      <c r="Q32" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="R32" s="16" t="s">
+      <c r="R32" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="S32" s="16" t="s">
+      <c r="S32" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="T32" s="16"/>
-      <c r="U32" s="16" t="s">
+      <c r="T32" s="13"/>
+      <c r="U32" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="V32" s="16" t="s">
+      <c r="V32" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="W32" s="16" t="s">
+      <c r="W32" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="X32" s="17" t="s">
+      <c r="X32" s="14" t="s">
         <v>11</v>
       </c>
       <c r="Y32" s="5"/>
@@ -6925,34 +6921,76 @@
         <v>0</v>
       </c>
       <c r="O36" s="13"/>
-      <c r="P36" s="24"/>
-      <c r="Q36" s="24"/>
-      <c r="R36" s="24"/>
-      <c r="S36" s="24"/>
-      <c r="T36" s="24"/>
-      <c r="U36" s="24"/>
-      <c r="V36" s="24"/>
-      <c r="W36" s="24"/>
-      <c r="X36" s="25"/>
+      <c r="P36" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q36" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="R36" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="S36" s="13"/>
+      <c r="T36" s="13">
+        <v>1</v>
+      </c>
+      <c r="U36" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="V36" s="13">
+        <v>0</v>
+      </c>
+      <c r="W36" s="13">
+        <v>0</v>
+      </c>
+      <c r="X36" s="14" t="s">
+        <v>3</v>
+      </c>
       <c r="Y36" s="5"/>
       <c r="Z36" s="5"/>
       <c r="AA36" s="5"/>
       <c r="AB36" s="5"/>
       <c r="AC36" s="5"/>
       <c r="AD36" s="5"/>
-      <c r="AE36" s="5"/>
-      <c r="AF36" s="5"/>
-      <c r="AG36" s="5"/>
-      <c r="AH36" s="5"/>
-      <c r="AI36" s="5"/>
-      <c r="AJ36" s="5"/>
-      <c r="AK36" s="5"/>
-      <c r="AL36" s="5"/>
-      <c r="AM36" s="5"/>
-      <c r="AN36" s="5"/>
-      <c r="AO36" s="5"/>
-      <c r="AP36" s="5"/>
-      <c r="AQ36" s="5"/>
+      <c r="AE36" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF36" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG36" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH36" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI36" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ36" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK36" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL36" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM36" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO36" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP36" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ36" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="AR36" s="5"/>
       <c r="AS36" s="5"/>
       <c r="AT36" s="5"/>
@@ -7046,27 +7084,67 @@
       <c r="C37" s="7">
         <v>7</v>
       </c>
-      <c r="D37" s="18"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
+      <c r="D37" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I37" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J37" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K37" s="19">
+        <v>0</v>
+      </c>
+      <c r="L37" s="19">
+        <v>0</v>
+      </c>
+      <c r="M37" s="19">
+        <v>0</v>
+      </c>
+      <c r="N37" s="19">
+        <v>0</v>
+      </c>
+      <c r="O37" s="19" t="s">
+        <v>36</v>
+      </c>
       <c r="P37" s="19"/>
-      <c r="Q37" s="19"/>
-      <c r="R37" s="19"/>
-      <c r="S37" s="19"/>
-      <c r="T37" s="19"/>
-      <c r="U37" s="19"/>
-      <c r="V37" s="19"/>
-      <c r="W37" s="19"/>
-      <c r="X37" s="20"/>
+      <c r="Q37" s="19">
+        <v>0</v>
+      </c>
+      <c r="R37" s="19">
+        <v>0</v>
+      </c>
+      <c r="S37" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="T37" s="19">
+        <v>0</v>
+      </c>
+      <c r="U37" s="19">
+        <v>0</v>
+      </c>
+      <c r="V37" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="W37" s="19">
+        <v>0</v>
+      </c>
+      <c r="X37" s="19">
+        <v>0</v>
+      </c>
       <c r="Y37" s="5"/>
       <c r="Z37" s="5"/>
       <c r="AA37" s="5"/>

</xml_diff>

<commit_message>
Tried to finesse number inputs - failed; fixed bugs
1 - added individual mutators for callbacks on MenuItem
2 - fixed bug in preference manager for uint8 vs short.
3 - tried to finesse number inputs on target editor - failed.
</commit_message>
<xml_diff>
--- a/Design/Screen-Layout.xlsx
+++ b/Design/Screen-Layout.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsasala/Development/Aquarius/Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F886CCE9-3A19-3E40-8D44-89E9CD7934C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE01CE0-EEBC-7741-AB77-5830770781E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12880" yWindow="2060" windowWidth="22960" windowHeight="17440" activeTab="3" xr2:uid="{0158349C-1CEF-DB49-8367-4BA8D3BA6996}"/>
+    <workbookView xWindow="12880" yWindow="2060" windowWidth="22960" windowHeight="17440" activeTab="4" xr2:uid="{0158349C-1CEF-DB49-8367-4BA8D3BA6996}"/>
   </bookViews>
   <sheets>
     <sheet name="Pixels" sheetId="1" r:id="rId1"/>
     <sheet name="Characters" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Button Layout" sheetId="4" r:id="rId3"/>
+    <sheet name="Constants" sheetId="3" r:id="rId4"/>
+    <sheet name="Scratch" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -442,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -497,9 +498,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -11086,6 +11084,1338 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FA56F5-0843-AB47-95D2-846E2A4461F9}">
+  <dimension ref="A1:DY64"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA31" sqref="AA31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="3.33203125" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:129" x14ac:dyDescent="0.2">
+      <c r="B1" s="23">
+        <v>0</v>
+      </c>
+      <c r="C1" s="23">
+        <f>B1+1</f>
+        <v>1</v>
+      </c>
+      <c r="D1" s="23">
+        <f t="shared" ref="D1:BO1" si="0">C1+1</f>
+        <v>2</v>
+      </c>
+      <c r="E1" s="23">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F1" s="23">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G1" s="23">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H1" s="23">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I1" s="23">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J1" s="23">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K1" s="23">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L1" s="23">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M1" s="23">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="N1" s="23">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="O1" s="23">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="P1" s="23">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q1" s="23">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="R1" s="23">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="S1" s="23">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="T1" s="23">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="U1" s="23">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="V1" s="23">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="W1" s="23">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="X1" s="23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="Y1" s="23">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="Z1" s="23">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="AA1" s="23">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="AB1" s="23">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="AC1" s="23">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="AD1" s="23">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="AE1" s="23">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="AF1" s="23">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="AG1" s="23">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="AH1" s="23">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="AI1" s="23">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="23">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="AK1" s="23">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="AL1" s="23">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="AM1" s="23">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="AN1" s="23">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="AO1" s="23">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="AP1" s="23">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="23">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="AR1" s="23">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="AS1" s="23">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="AT1" s="23">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="AU1" s="23">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="AV1" s="23">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="AW1" s="23">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="AX1" s="23">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="AY1" s="23">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="23">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="BA1" s="23">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="BB1" s="23">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="BC1" s="23">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="BD1" s="23">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="BE1" s="23">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="BF1" s="23">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="BG1" s="23">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="BH1" s="23">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="BI1" s="23">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="BJ1" s="23">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="BK1" s="23">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="BL1" s="23">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="BM1" s="23">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="BN1" s="23">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="BO1" s="23">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="BP1" s="23">
+        <f t="shared" ref="BP1:DY1" si="1">BO1+1</f>
+        <v>66</v>
+      </c>
+      <c r="BQ1" s="23">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="BR1" s="23">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="BS1" s="23">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="BT1" s="23">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="BU1" s="23">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="BV1" s="23">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="BW1" s="23">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="BX1" s="23">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="BY1" s="23">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="BZ1" s="23">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="CA1" s="23">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="CB1" s="23">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="CC1" s="23">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="CD1" s="23">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="CE1" s="23">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="CF1" s="23">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="CG1" s="23">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="CH1" s="23">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="CI1" s="23">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="CJ1" s="23">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="CK1" s="23">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="CL1" s="23">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="CM1" s="23">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="CN1" s="23">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="CO1" s="23">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="CP1" s="23">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="CQ1" s="23">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="CR1" s="23">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="CS1" s="23">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="CT1" s="23">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="CU1" s="23">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="CV1" s="23">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="CW1" s="23">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="CX1" s="23">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="CY1" s="23">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+      <c r="CZ1" s="23">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="DA1" s="23">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="DB1" s="23">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="DC1" s="23">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="DD1" s="23">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="DE1" s="23">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="DF1" s="23">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="DG1" s="23">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="DH1" s="23">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="DI1" s="23">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="DJ1" s="23">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="DK1" s="23">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="DL1" s="23">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="DM1" s="23">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+      <c r="DN1" s="23">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="DO1" s="23">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="DP1" s="23">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="DQ1" s="23">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+      <c r="DR1" s="23">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="DS1" s="23">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="DT1" s="23">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="DU1" s="23">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="DV1" s="23">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="DW1" s="23">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="DX1" s="23">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="DY1" s="23">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:129" x14ac:dyDescent="0.2">
+      <c r="A2" s="23">
+        <v>0</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="T2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="W2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="X2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC2" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:129" x14ac:dyDescent="0.2">
+      <c r="A3" s="23">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD3" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:129" x14ac:dyDescent="0.2">
+      <c r="A4" s="23">
+        <f t="shared" ref="A4:A64" si="2">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="25"/>
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="25"/>
+      <c r="AE4" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:129" x14ac:dyDescent="0.2">
+      <c r="A5" s="23">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="25"/>
+      <c r="AB5" s="25"/>
+      <c r="AC5" s="25"/>
+      <c r="AE5" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:129" x14ac:dyDescent="0.2">
+      <c r="A6" s="23">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="25"/>
+      <c r="X6" s="25"/>
+      <c r="Y6" s="25"/>
+      <c r="Z6" s="25"/>
+      <c r="AA6" s="25"/>
+      <c r="AB6" s="25"/>
+      <c r="AC6" s="25"/>
+      <c r="AE6" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:129" x14ac:dyDescent="0.2">
+      <c r="A7" s="23">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="24"/>
+      <c r="W7" s="25"/>
+      <c r="X7" s="25"/>
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="25"/>
+      <c r="AA7" s="25"/>
+      <c r="AB7" s="25"/>
+      <c r="AC7" s="25"/>
+      <c r="AE7" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:129" x14ac:dyDescent="0.2">
+      <c r="A8" s="23">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="25"/>
+      <c r="X8" s="25"/>
+      <c r="Y8" s="25"/>
+      <c r="Z8" s="25"/>
+      <c r="AA8" s="25"/>
+      <c r="AB8" s="25"/>
+      <c r="AC8" s="25"/>
+      <c r="AE8" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:129" x14ac:dyDescent="0.2">
+      <c r="A9" s="23">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="25"/>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
+      <c r="AA9" s="25"/>
+      <c r="AB9" s="25"/>
+      <c r="AC9" s="25"/>
+      <c r="AE9" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:129" x14ac:dyDescent="0.2">
+      <c r="A10" s="23">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="25"/>
+      <c r="X10" s="25"/>
+      <c r="Y10" s="25"/>
+      <c r="Z10" s="25"/>
+      <c r="AA10" s="25"/>
+      <c r="AB10" s="25"/>
+      <c r="AC10" s="25"/>
+      <c r="AE10" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:129" x14ac:dyDescent="0.2">
+      <c r="A11" s="23">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="25"/>
+      <c r="X11" s="25"/>
+      <c r="Y11" s="25"/>
+      <c r="Z11" s="25"/>
+      <c r="AA11" s="25"/>
+      <c r="AB11" s="25"/>
+      <c r="AC11" s="25"/>
+      <c r="AE11" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:129" x14ac:dyDescent="0.2">
+      <c r="A12" s="23">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD12" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:129" x14ac:dyDescent="0.2">
+      <c r="A13" s="23">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="M13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="N13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="O13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="P13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="R13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="S13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="T13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="U13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="V13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="W13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="X13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC13" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:129" x14ac:dyDescent="0.2">
+      <c r="A14" s="23">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:129" x14ac:dyDescent="0.2">
+      <c r="A15" s="23">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:129" x14ac:dyDescent="0.2">
+      <c r="A16" s="23">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="23">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="23">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="23">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="23">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="23">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="23">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="23">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="23">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="23">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="23">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="23">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="23">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="23">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="23">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="23">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="23">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="23">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="23">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="23">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="23">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="23">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="23">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="23">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="23">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="23">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="23">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="23">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="23">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="23">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="23">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="23">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="23">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="23">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="23">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="23">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="23">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="23">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="23">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="23">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="23">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="23">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="23">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="23">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="23">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="23">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="23">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="23">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="23">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A1A604-8CBD-8942-AD0D-E85BA7A9EB6D}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -11153,1355 +12483,287 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FA56F5-0843-AB47-95D2-846E2A4461F9}">
-  <dimension ref="A1:DY64"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FB5F1D7-BA4F-6D46-859B-81C53B28AF51}">
+  <dimension ref="B2:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA31" sqref="AA31"/>
+      <selection activeCell="D4" sqref="D4:D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="3.33203125" style="23"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:129" x14ac:dyDescent="0.2">
-      <c r="B1" s="23">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="C1" s="23">
-        <f>B1+1</f>
+      <c r="C3">
+        <f>B3+1</f>
         <v>1</v>
       </c>
-      <c r="D1" s="23">
-        <f t="shared" ref="D1:BO1" si="0">C1+1</f>
+      <c r="D3">
+        <f>B3+2</f>
         <v>2</v>
       </c>
-      <c r="E1" s="23">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <f>B3+1</f>
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C21" si="0">B4+1</f>
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D21" si="1">B4+2</f>
         <v>3</v>
       </c>
-      <c r="F1" s="23">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <f t="shared" ref="B5:B21" si="2">B4+1</f>
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G1" s="23">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="H1" s="23">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I1" s="23">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J1" s="23">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="K1" s="23">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="L1" s="23">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="M1" s="23">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="N1" s="23">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="O1" s="23">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="P1" s="23">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="Q1" s="23">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="R1" s="23">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="S1" s="23">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="T1" s="23">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="U1" s="23">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="V1" s="23">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
         <v>20</v>
-      </c>
-      <c r="W1" s="23">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="X1" s="23">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="Y1" s="23">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="Z1" s="23">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="AA1" s="23">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="AB1" s="23">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="AC1" s="23">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="AD1" s="23">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="AE1" s="23">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="AF1" s="23">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="AG1" s="23">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="AH1" s="23">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="AI1" s="23">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="AJ1" s="23">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="AK1" s="23">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="AL1" s="23">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="AM1" s="23">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="AN1" s="23">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="AO1" s="23">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="AP1" s="23">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="AQ1" s="23">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="AR1" s="23">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="AS1" s="23">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="AT1" s="23">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="AU1" s="23">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="AV1" s="23">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="AW1" s="23">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="AX1" s="23">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="AY1" s="23">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="AZ1" s="23">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="BA1" s="23">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="BB1" s="23">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="BC1" s="23">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="BD1" s="23">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="BE1" s="23">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="BF1" s="23">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="BG1" s="23">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="BH1" s="23">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="BI1" s="23">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="BJ1" s="23">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="BK1" s="23">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="BL1" s="23">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="BM1" s="23">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="BN1" s="23">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="BO1" s="23">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="BP1" s="23">
-        <f t="shared" ref="BP1:DY1" si="1">BO1+1</f>
-        <v>66</v>
-      </c>
-      <c r="BQ1" s="23">
-        <f t="shared" si="1"/>
-        <v>67</v>
-      </c>
-      <c r="BR1" s="23">
-        <f t="shared" si="1"/>
-        <v>68</v>
-      </c>
-      <c r="BS1" s="23">
-        <f t="shared" si="1"/>
-        <v>69</v>
-      </c>
-      <c r="BT1" s="23">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="BU1" s="23">
-        <f t="shared" si="1"/>
-        <v>71</v>
-      </c>
-      <c r="BV1" s="23">
-        <f t="shared" si="1"/>
-        <v>72</v>
-      </c>
-      <c r="BW1" s="23">
-        <f t="shared" si="1"/>
-        <v>73</v>
-      </c>
-      <c r="BX1" s="23">
-        <f t="shared" si="1"/>
-        <v>74</v>
-      </c>
-      <c r="BY1" s="23">
-        <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-      <c r="BZ1" s="23">
-        <f t="shared" si="1"/>
-        <v>76</v>
-      </c>
-      <c r="CA1" s="23">
-        <f t="shared" si="1"/>
-        <v>77</v>
-      </c>
-      <c r="CB1" s="23">
-        <f t="shared" si="1"/>
-        <v>78</v>
-      </c>
-      <c r="CC1" s="23">
-        <f t="shared" si="1"/>
-        <v>79</v>
-      </c>
-      <c r="CD1" s="23">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="CE1" s="23">
-        <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="CF1" s="23">
-        <f t="shared" si="1"/>
-        <v>82</v>
-      </c>
-      <c r="CG1" s="23">
-        <f t="shared" si="1"/>
-        <v>83</v>
-      </c>
-      <c r="CH1" s="23">
-        <f t="shared" si="1"/>
-        <v>84</v>
-      </c>
-      <c r="CI1" s="23">
-        <f t="shared" si="1"/>
-        <v>85</v>
-      </c>
-      <c r="CJ1" s="23">
-        <f t="shared" si="1"/>
-        <v>86</v>
-      </c>
-      <c r="CK1" s="23">
-        <f t="shared" si="1"/>
-        <v>87</v>
-      </c>
-      <c r="CL1" s="23">
-        <f t="shared" si="1"/>
-        <v>88</v>
-      </c>
-      <c r="CM1" s="23">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="CN1" s="23">
-        <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="CO1" s="23">
-        <f t="shared" si="1"/>
-        <v>91</v>
-      </c>
-      <c r="CP1" s="23">
-        <f t="shared" si="1"/>
-        <v>92</v>
-      </c>
-      <c r="CQ1" s="23">
-        <f t="shared" si="1"/>
-        <v>93</v>
-      </c>
-      <c r="CR1" s="23">
-        <f t="shared" si="1"/>
-        <v>94</v>
-      </c>
-      <c r="CS1" s="23">
-        <f t="shared" si="1"/>
-        <v>95</v>
-      </c>
-      <c r="CT1" s="23">
-        <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-      <c r="CU1" s="23">
-        <f t="shared" si="1"/>
-        <v>97</v>
-      </c>
-      <c r="CV1" s="23">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-      <c r="CW1" s="23">
-        <f t="shared" si="1"/>
-        <v>99</v>
-      </c>
-      <c r="CX1" s="23">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="CY1" s="23">
-        <f t="shared" si="1"/>
-        <v>101</v>
-      </c>
-      <c r="CZ1" s="23">
-        <f t="shared" si="1"/>
-        <v>102</v>
-      </c>
-      <c r="DA1" s="23">
-        <f t="shared" si="1"/>
-        <v>103</v>
-      </c>
-      <c r="DB1" s="23">
-        <f t="shared" si="1"/>
-        <v>104</v>
-      </c>
-      <c r="DC1" s="23">
-        <f t="shared" si="1"/>
-        <v>105</v>
-      </c>
-      <c r="DD1" s="23">
-        <f t="shared" si="1"/>
-        <v>106</v>
-      </c>
-      <c r="DE1" s="23">
-        <f t="shared" si="1"/>
-        <v>107</v>
-      </c>
-      <c r="DF1" s="23">
-        <f t="shared" si="1"/>
-        <v>108</v>
-      </c>
-      <c r="DG1" s="23">
-        <f t="shared" si="1"/>
-        <v>109</v>
-      </c>
-      <c r="DH1" s="23">
-        <f t="shared" si="1"/>
-        <v>110</v>
-      </c>
-      <c r="DI1" s="23">
-        <f t="shared" si="1"/>
-        <v>111</v>
-      </c>
-      <c r="DJ1" s="23">
-        <f t="shared" si="1"/>
-        <v>112</v>
-      </c>
-      <c r="DK1" s="23">
-        <f t="shared" si="1"/>
-        <v>113</v>
-      </c>
-      <c r="DL1" s="23">
-        <f t="shared" si="1"/>
-        <v>114</v>
-      </c>
-      <c r="DM1" s="23">
-        <f t="shared" si="1"/>
-        <v>115</v>
-      </c>
-      <c r="DN1" s="23">
-        <f t="shared" si="1"/>
-        <v>116</v>
-      </c>
-      <c r="DO1" s="23">
-        <f t="shared" si="1"/>
-        <v>117</v>
-      </c>
-      <c r="DP1" s="23">
-        <f t="shared" si="1"/>
-        <v>118</v>
-      </c>
-      <c r="DQ1" s="23">
-        <f t="shared" si="1"/>
-        <v>119</v>
-      </c>
-      <c r="DR1" s="23">
-        <f t="shared" si="1"/>
-        <v>120</v>
-      </c>
-      <c r="DS1" s="23">
-        <f t="shared" si="1"/>
-        <v>121</v>
-      </c>
-      <c r="DT1" s="23">
-        <f t="shared" si="1"/>
-        <v>122</v>
-      </c>
-      <c r="DU1" s="23">
-        <f t="shared" si="1"/>
-        <v>123</v>
-      </c>
-      <c r="DV1" s="23">
-        <f t="shared" si="1"/>
-        <v>124</v>
-      </c>
-      <c r="DW1" s="23">
-        <f t="shared" si="1"/>
-        <v>125</v>
-      </c>
-      <c r="DX1" s="23">
-        <f t="shared" si="1"/>
-        <v>126</v>
-      </c>
-      <c r="DY1" s="23">
-        <f t="shared" si="1"/>
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:129" x14ac:dyDescent="0.2">
-      <c r="A2" s="23">
-        <v>0</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="K2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="M2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="N2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="O2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="P2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="R2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="S2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="T2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="U2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="V2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="W2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="X2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
-    </row>
-    <row r="3" spans="1:129" x14ac:dyDescent="0.2">
-      <c r="A3" s="23">
-        <f>A2+1</f>
-        <v>1</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="AD3" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:129" x14ac:dyDescent="0.2">
-      <c r="A4" s="23">
-        <f t="shared" ref="A4:A64" si="2">A3+1</f>
-        <v>2</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="25"/>
-      <c r="V4" s="25"/>
-      <c r="W4" s="26"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="26"/>
-      <c r="Z4" s="26"/>
-      <c r="AA4" s="26"/>
-      <c r="AB4" s="26"/>
-      <c r="AC4" s="26"/>
-      <c r="AE4" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:129" x14ac:dyDescent="0.2">
-      <c r="A5" s="23">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
-      <c r="V5" s="25"/>
-      <c r="W5" s="26"/>
-      <c r="X5" s="26"/>
-      <c r="Y5" s="26"/>
-      <c r="Z5" s="26"/>
-      <c r="AA5" s="26"/>
-      <c r="AB5" s="26"/>
-      <c r="AC5" s="26"/>
-      <c r="AE5" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:129" x14ac:dyDescent="0.2">
-      <c r="A6" s="23">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="25"/>
-      <c r="V6" s="25"/>
-      <c r="W6" s="26"/>
-      <c r="X6" s="26"/>
-      <c r="Y6" s="26"/>
-      <c r="Z6" s="26"/>
-      <c r="AA6" s="26"/>
-      <c r="AB6" s="26"/>
-      <c r="AC6" s="26"/>
-      <c r="AE6" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:129" x14ac:dyDescent="0.2">
-      <c r="A7" s="23">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="25"/>
-      <c r="V7" s="25"/>
-      <c r="W7" s="26"/>
-      <c r="X7" s="26"/>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="26"/>
-      <c r="AA7" s="26"/>
-      <c r="AB7" s="26"/>
-      <c r="AC7" s="26"/>
-      <c r="AE7" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:129" x14ac:dyDescent="0.2">
-      <c r="A8" s="23">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="25"/>
-      <c r="V8" s="25"/>
-      <c r="W8" s="26"/>
-      <c r="X8" s="26"/>
-      <c r="Y8" s="26"/>
-      <c r="Z8" s="26"/>
-      <c r="AA8" s="26"/>
-      <c r="AB8" s="26"/>
-      <c r="AC8" s="26"/>
-      <c r="AE8" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:129" x14ac:dyDescent="0.2">
-      <c r="A9" s="23">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="25"/>
-      <c r="V9" s="25"/>
-      <c r="W9" s="26"/>
-      <c r="X9" s="26"/>
-      <c r="Y9" s="26"/>
-      <c r="Z9" s="26"/>
-      <c r="AA9" s="26"/>
-      <c r="AB9" s="26"/>
-      <c r="AC9" s="26"/>
-      <c r="AE9" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:129" x14ac:dyDescent="0.2">
-      <c r="A10" s="23">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="25"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="26"/>
-      <c r="X10" s="26"/>
-      <c r="Y10" s="26"/>
-      <c r="Z10" s="26"/>
-      <c r="AA10" s="26"/>
-      <c r="AB10" s="26"/>
-      <c r="AC10" s="26"/>
-      <c r="AE10" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:129" x14ac:dyDescent="0.2">
-      <c r="A11" s="23">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="25"/>
-      <c r="V11" s="25"/>
-      <c r="W11" s="26"/>
-      <c r="X11" s="26"/>
-      <c r="Y11" s="26"/>
-      <c r="Z11" s="26"/>
-      <c r="AA11" s="26"/>
-      <c r="AB11" s="26"/>
-      <c r="AC11" s="26"/>
-      <c r="AE11" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:129" x14ac:dyDescent="0.2">
-      <c r="A12" s="23">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD12" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:129" x14ac:dyDescent="0.2">
-      <c r="A13" s="23">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="K13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="M13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="N13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="O13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="P13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="R13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="S13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="T13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="U13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="V13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="W13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="X13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB13" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC13" s="24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:129" x14ac:dyDescent="0.2">
-      <c r="A14" s="23">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:129" x14ac:dyDescent="0.2">
-      <c r="A15" s="23">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:129" x14ac:dyDescent="0.2">
-      <c r="A16" s="23">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="23">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="23">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="23">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="23">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="23">
-        <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="23">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="23">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="23">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="23">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="23">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="23">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="23">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="23">
-        <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="23">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="23">
-        <f t="shared" si="2"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="23">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="23">
-        <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="23">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="23">
-        <f t="shared" si="2"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="23">
-        <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="23">
-        <f t="shared" si="2"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="23">
-        <f t="shared" si="2"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="23">
-        <f t="shared" si="2"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="23">
-        <f t="shared" si="2"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="23">
-        <f t="shared" si="2"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="23">
-        <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="23">
-        <f t="shared" si="2"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="23">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="23">
-        <f t="shared" si="2"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="23">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="23">
-        <f t="shared" si="2"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="23">
-        <f t="shared" si="2"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="23">
-        <f t="shared" si="2"/>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="23">
-        <f t="shared" si="2"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="23">
-        <f t="shared" si="2"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="23">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="23">
-        <f t="shared" si="2"/>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="23">
-        <f t="shared" si="2"/>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="23">
-        <f t="shared" si="2"/>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="23">
-        <f t="shared" si="2"/>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="23">
-        <f t="shared" si="2"/>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="23">
-        <f t="shared" si="2"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="23">
-        <f t="shared" si="2"/>
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="23">
-        <f t="shared" si="2"/>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="23">
-        <f t="shared" si="2"/>
-        <v>59</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="23">
-        <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="23">
-        <f t="shared" si="2"/>
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="23">
-        <f t="shared" si="2"/>
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on target create.
</commit_message>
<xml_diff>
--- a/Design/Screen-Layout.xlsx
+++ b/Design/Screen-Layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsasala/Development/Aquarius/Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE01CE0-EEBC-7741-AB77-5830770781E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381D10DA-C919-2E4D-8AD9-3EC902C2A201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12880" yWindow="2060" windowWidth="22960" windowHeight="17440" activeTab="4" xr2:uid="{0158349C-1CEF-DB49-8367-4BA8D3BA6996}"/>
+    <workbookView xWindow="12880" yWindow="2060" windowWidth="22960" windowHeight="17440" activeTab="1" xr2:uid="{0158349C-1CEF-DB49-8367-4BA8D3BA6996}"/>
   </bookViews>
   <sheets>
     <sheet name="Pixels" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="43">
   <si>
     <t>W</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Mod9</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>r</t>
   </si>
 </sst>
 </file>
@@ -443,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -504,6 +513,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -823,7 +844,7 @@
   <dimension ref="A1:DY64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="A1:DY64"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1861,8 +1882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE90A50E-CDCD-574E-8857-69572E52BB25}">
   <dimension ref="A1:EA66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P38" sqref="P38"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="AT33" sqref="AT33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7672,7 +7693,7 @@
       <c r="DZ40" s="5"/>
       <c r="EA40" s="5"/>
     </row>
-    <row r="41" spans="3:131" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:131" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
@@ -7804,28 +7825,70 @@
       <c r="EA41" s="5"/>
     </row>
     <row r="42" spans="3:131" x14ac:dyDescent="0.2">
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="5"/>
-      <c r="O42" s="5"/>
-      <c r="P42" s="5"/>
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
-      <c r="U42" s="5"/>
-      <c r="V42" s="5"/>
-      <c r="W42" s="5"/>
-      <c r="X42" s="5"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="26">
+        <v>0</v>
+      </c>
+      <c r="E42" s="26">
+        <v>1</v>
+      </c>
+      <c r="F42" s="26">
+        <v>2</v>
+      </c>
+      <c r="G42" s="26">
+        <v>3</v>
+      </c>
+      <c r="H42" s="26">
+        <v>4</v>
+      </c>
+      <c r="I42" s="26">
+        <v>5</v>
+      </c>
+      <c r="J42" s="26">
+        <v>6</v>
+      </c>
+      <c r="K42" s="26">
+        <v>7</v>
+      </c>
+      <c r="L42" s="26">
+        <v>8</v>
+      </c>
+      <c r="M42" s="26">
+        <v>9</v>
+      </c>
+      <c r="N42" s="26">
+        <v>10</v>
+      </c>
+      <c r="O42" s="26">
+        <v>11</v>
+      </c>
+      <c r="P42" s="26">
+        <v>12</v>
+      </c>
+      <c r="Q42" s="26">
+        <v>13</v>
+      </c>
+      <c r="R42" s="26">
+        <v>14</v>
+      </c>
+      <c r="S42" s="26">
+        <v>15</v>
+      </c>
+      <c r="T42" s="26">
+        <v>16</v>
+      </c>
+      <c r="U42" s="26">
+        <v>17</v>
+      </c>
+      <c r="V42" s="26">
+        <v>18</v>
+      </c>
+      <c r="W42" s="26">
+        <v>19</v>
+      </c>
+      <c r="X42" s="27">
+        <v>20</v>
+      </c>
       <c r="Y42" s="5"/>
       <c r="Z42" s="5"/>
       <c r="AA42" s="5"/>
@@ -7935,28 +7998,30 @@
       <c r="EA42" s="5"/>
     </row>
     <row r="43" spans="3:131" x14ac:dyDescent="0.2">
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5"/>
-      <c r="N43" s="5"/>
-      <c r="O43" s="5"/>
-      <c r="P43" s="5"/>
-      <c r="Q43" s="5"/>
-      <c r="R43" s="5"/>
-      <c r="S43" s="5"/>
-      <c r="T43" s="5"/>
-      <c r="U43" s="5"/>
-      <c r="V43" s="5"/>
-      <c r="W43" s="5"/>
-      <c r="X43" s="5"/>
+      <c r="C43" s="28">
+        <v>0</v>
+      </c>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="13"/>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="13"/>
+      <c r="S43" s="13"/>
+      <c r="T43" s="13"/>
+      <c r="U43" s="13"/>
+      <c r="V43" s="13"/>
+      <c r="W43" s="13"/>
+      <c r="X43" s="14"/>
       <c r="Y43" s="5"/>
       <c r="Z43" s="5"/>
       <c r="AA43" s="5"/>
@@ -8066,28 +8131,48 @@
       <c r="EA43" s="5"/>
     </row>
     <row r="44" spans="3:131" x14ac:dyDescent="0.2">
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="5"/>
-      <c r="P44" s="5"/>
-      <c r="Q44" s="5"/>
-      <c r="R44" s="5"/>
-      <c r="S44" s="5"/>
-      <c r="T44" s="5"/>
-      <c r="U44" s="5"/>
-      <c r="V44" s="5"/>
-      <c r="W44" s="5"/>
-      <c r="X44" s="5"/>
+      <c r="C44" s="28">
+        <v>1</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I44" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J44" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="K44" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="N44" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="O44" s="13"/>
+      <c r="P44" s="13"/>
+      <c r="Q44" s="13"/>
+      <c r="R44" s="13"/>
+      <c r="S44" s="13"/>
+      <c r="T44" s="13"/>
+      <c r="U44" s="13"/>
+      <c r="V44" s="13"/>
+      <c r="W44" s="13"/>
+      <c r="X44" s="14"/>
       <c r="Y44" s="5"/>
       <c r="Z44" s="5"/>
       <c r="AA44" s="5"/>
@@ -8197,28 +8282,30 @@
       <c r="EA44" s="5"/>
     </row>
     <row r="45" spans="3:131" x14ac:dyDescent="0.2">
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="5"/>
-      <c r="T45" s="5"/>
-      <c r="U45" s="5"/>
-      <c r="V45" s="5"/>
-      <c r="W45" s="5"/>
-      <c r="X45" s="5"/>
+      <c r="C45" s="28">
+        <v>2</v>
+      </c>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
+      <c r="N45" s="13"/>
+      <c r="O45" s="13"/>
+      <c r="P45" s="13"/>
+      <c r="Q45" s="13"/>
+      <c r="R45" s="13"/>
+      <c r="S45" s="13"/>
+      <c r="T45" s="13"/>
+      <c r="U45" s="13"/>
+      <c r="V45" s="13"/>
+      <c r="W45" s="13"/>
+      <c r="X45" s="14"/>
       <c r="Y45" s="5"/>
       <c r="Z45" s="5"/>
       <c r="AA45" s="5"/>
@@ -8328,28 +8415,30 @@
       <c r="EA45" s="5"/>
     </row>
     <row r="46" spans="3:131" x14ac:dyDescent="0.2">
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5"/>
-      <c r="O46" s="5"/>
-      <c r="P46" s="5"/>
-      <c r="Q46" s="5"/>
-      <c r="R46" s="5"/>
-      <c r="S46" s="5"/>
-      <c r="T46" s="5"/>
-      <c r="U46" s="5"/>
-      <c r="V46" s="5"/>
-      <c r="W46" s="5"/>
-      <c r="X46" s="5"/>
+      <c r="C46" s="28">
+        <v>3</v>
+      </c>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="13"/>
+      <c r="S46" s="13"/>
+      <c r="T46" s="13"/>
+      <c r="U46" s="13"/>
+      <c r="V46" s="13"/>
+      <c r="W46" s="13"/>
+      <c r="X46" s="14"/>
       <c r="Y46" s="5"/>
       <c r="Z46" s="5"/>
       <c r="AA46" s="5"/>
@@ -8459,28 +8548,30 @@
       <c r="EA46" s="5"/>
     </row>
     <row r="47" spans="3:131" x14ac:dyDescent="0.2">
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="5"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="5"/>
-      <c r="R47" s="5"/>
-      <c r="S47" s="5"/>
-      <c r="T47" s="5"/>
-      <c r="U47" s="5"/>
-      <c r="V47" s="5"/>
-      <c r="W47" s="5"/>
-      <c r="X47" s="5"/>
+      <c r="C47" s="28">
+        <v>4</v>
+      </c>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="13"/>
+      <c r="P47" s="13"/>
+      <c r="Q47" s="13"/>
+      <c r="R47" s="13"/>
+      <c r="S47" s="13"/>
+      <c r="T47" s="13"/>
+      <c r="U47" s="13"/>
+      <c r="V47" s="13"/>
+      <c r="W47" s="13"/>
+      <c r="X47" s="14"/>
       <c r="Y47" s="5"/>
       <c r="Z47" s="5"/>
       <c r="AA47" s="5"/>
@@ -8590,28 +8681,30 @@
       <c r="EA47" s="5"/>
     </row>
     <row r="48" spans="3:131" x14ac:dyDescent="0.2">
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
-      <c r="L48" s="5"/>
-      <c r="M48" s="5"/>
-      <c r="N48" s="5"/>
-      <c r="O48" s="5"/>
-      <c r="P48" s="5"/>
-      <c r="Q48" s="5"/>
-      <c r="R48" s="5"/>
-      <c r="S48" s="5"/>
-      <c r="T48" s="5"/>
-      <c r="U48" s="5"/>
-      <c r="V48" s="5"/>
-      <c r="W48" s="5"/>
-      <c r="X48" s="5"/>
+      <c r="C48" s="28">
+        <v>5</v>
+      </c>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
+      <c r="N48" s="13"/>
+      <c r="O48" s="13"/>
+      <c r="P48" s="13"/>
+      <c r="Q48" s="13"/>
+      <c r="R48" s="13"/>
+      <c r="S48" s="13"/>
+      <c r="T48" s="13"/>
+      <c r="U48" s="13"/>
+      <c r="V48" s="13"/>
+      <c r="W48" s="13"/>
+      <c r="X48" s="14"/>
       <c r="Y48" s="5"/>
       <c r="Z48" s="5"/>
       <c r="AA48" s="5"/>
@@ -8721,28 +8814,30 @@
       <c r="EA48" s="5"/>
     </row>
     <row r="49" spans="3:131" x14ac:dyDescent="0.2">
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
-      <c r="N49" s="5"/>
-      <c r="O49" s="5"/>
-      <c r="P49" s="5"/>
-      <c r="Q49" s="5"/>
-      <c r="R49" s="5"/>
-      <c r="S49" s="5"/>
-      <c r="T49" s="5"/>
-      <c r="U49" s="5"/>
-      <c r="V49" s="5"/>
-      <c r="W49" s="5"/>
-      <c r="X49" s="5"/>
+      <c r="C49" s="28">
+        <v>6</v>
+      </c>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="13"/>
+      <c r="P49" s="13"/>
+      <c r="Q49" s="13"/>
+      <c r="R49" s="13"/>
+      <c r="S49" s="13"/>
+      <c r="T49" s="13"/>
+      <c r="U49" s="13"/>
+      <c r="V49" s="13"/>
+      <c r="W49" s="13"/>
+      <c r="X49" s="14"/>
       <c r="Y49" s="5"/>
       <c r="Z49" s="5"/>
       <c r="AA49" s="5"/>
@@ -8851,29 +8946,31 @@
       <c r="DZ49" s="5"/>
       <c r="EA49" s="5"/>
     </row>
-    <row r="50" spans="3:131" x14ac:dyDescent="0.2">
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="5"/>
-      <c r="L50" s="5"/>
-      <c r="M50" s="5"/>
-      <c r="N50" s="5"/>
-      <c r="O50" s="5"/>
-      <c r="P50" s="5"/>
-      <c r="Q50" s="5"/>
-      <c r="R50" s="5"/>
-      <c r="S50" s="5"/>
-      <c r="T50" s="5"/>
-      <c r="U50" s="5"/>
-      <c r="V50" s="5"/>
-      <c r="W50" s="5"/>
-      <c r="X50" s="5"/>
+    <row r="50" spans="3:131" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="29">
+        <v>7</v>
+      </c>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19"/>
+      <c r="P50" s="19"/>
+      <c r="Q50" s="19"/>
+      <c r="R50" s="19"/>
+      <c r="S50" s="19"/>
+      <c r="T50" s="19"/>
+      <c r="U50" s="19"/>
+      <c r="V50" s="19"/>
+      <c r="W50" s="19"/>
+      <c r="X50" s="20"/>
       <c r="Y50" s="5"/>
       <c r="Z50" s="5"/>
       <c r="AA50" s="5"/>
@@ -11088,7 +11185,7 @@
   <dimension ref="A1:DY64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA31" sqref="AA31"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12485,23 +12582,29 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FB5F1D7-BA4F-6D46-859B-81C53B28AF51}">
-  <dimension ref="B2:D21"/>
+  <dimension ref="B2:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>0</v>
       </c>
@@ -12510,260 +12613,639 @@
         <v>1</v>
       </c>
       <c r="D3">
+        <f t="shared" ref="D3:D10" si="0">MOD(C3,10)</f>
+        <v>1</v>
+      </c>
+      <c r="E3">
         <f>B3+2</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <f t="shared" ref="F3:F21" si="1">MOD(E3,10)</f>
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>-1</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I21" si="2">MOD(H3,10)</f>
+        <v>9</v>
+      </c>
+      <c r="J3">
+        <f>10+H3</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4">
         <f>B3+1</f>
         <v>1</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C21" si="0">B4+1</f>
+        <f t="shared" ref="C4:C21" si="3">B4+1</f>
         <v>2</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D21" si="1">B4+2</f>
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E21" si="4">B4+2</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <f>H3-1</f>
+        <v>-2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J21" si="5">10+H4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5">
-        <f t="shared" ref="B5:B21" si="2">B4+1</f>
+        <f t="shared" ref="B5:B21" si="6">B4+1</f>
         <v>2</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H21" si="7">H4-1</f>
+        <v>-3</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="7"/>
+        <v>-4</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="7"/>
+        <v>-5</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="7"/>
+        <v>-6</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="7"/>
+        <v>-7</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="7"/>
+        <v>-8</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f>MOD(C11,10)</f>
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="7"/>
+        <v>-9</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D12:D21" si="8">MOD(C12,10)</f>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="7"/>
+        <v>-10</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="7"/>
+        <v>-11</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="7"/>
+        <v>-12</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="5"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="7"/>
+        <v>-13</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="5"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="7"/>
+        <v>-14</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="5"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="7"/>
+        <v>-15</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="5"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="7"/>
+        <v>-16</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="5"/>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="7"/>
+        <v>-17</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="5"/>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="7"/>
+        <v>-18</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="5"/>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="4"/>
         <v>20</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="7"/>
+        <v>-19</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="5"/>
+        <v>-9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>